<commit_message>
keyboard and display interfaces
</commit_message>
<xml_diff>
--- a/TextRadioDiagram.xlsx
+++ b/TextRadioDiagram.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RayMetz100\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RayMetz100\Documents\GitHub\TextWalkieTalkie\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -639,8 +639,27 @@
                 <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
             </a:rPr>
+            <a:t>-Input Interface</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
             <a:t>-2.5" LCD</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1098,6 +1117,17 @@
               </a:solidFill>
             </a:rPr>
             <a:t>-2.5 inches wide</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>-Keyboard output interface</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -1661,7 +1691,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>